<commit_message>
added 15 threads test
</commit_message>
<xml_diff>
--- a/performance_tests.xlsx
+++ b/performance_tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\FILIPPO\UNIVERSITA\MAGISTRALE\PROGRAMMAZIONE_CONCORRENTE_DISTRIBUITA\pcd-assignment-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DC4C22-5BD8-43B2-8E48-607711AD9F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C10A36-9F67-4265-BFFA-DB0CA427673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8F27FFE-6F90-43A3-9F82-231864281E9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>SEQUENZIALE</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>15 thread</t>
   </si>
 </sst>
 </file>
@@ -323,6 +326,24 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$B$3:$D$3</c:f>
@@ -398,7 +419,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$G$5:$I$5</c:f>
+              <c:f>Foglio1!$G$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -471,7 +492,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$G$4:$I$4</c:f>
+              <c:f>Foglio1!$G$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -544,7 +565,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$G$3:$I$3</c:f>
+              <c:f>Foglio1!$G$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -564,6 +585,96 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2C90-4504-9E13-6D8020375488}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>15 thread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="90000"/>
+                    <a:lumOff val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$G$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4775-4431-967A-30F875EADAEB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -970,6 +1081,24 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$L$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$B$3:$D$3</c:f>
@@ -1000,7 +1129,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$5</c:f>
+              <c:f>Foglio1!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1035,7 +1164,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:f>Foglio1!$L$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1053,7 +1182,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$5:$N$5</c:f>
+              <c:f>Foglio1!$L$6:$N$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1081,7 +1210,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$4</c:f>
+              <c:f>Foglio1!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1116,7 +1245,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:f>Foglio1!$L$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1134,7 +1263,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$L$4:$N$4</c:f>
+              <c:f>Foglio1!$L$5:$N$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1158,11 +1287,11 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$K$3</c:f>
+              <c:f>Foglio1!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1195,6 +1324,96 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$L$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$L$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F003-4C51-8A78-E2F45B7518DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>15 thread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="90000"/>
+                    <a:lumOff val="10000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:dPt>
             <c:idx val="2"/>
             <c:marker>
@@ -1202,11 +1421,17 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:srgbClr val="C00000"/>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="90000"/>
+                    <a:lumOff val="10000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="C00000"/>
+                    <a:schemeClr val="tx2">
+                      <a:lumMod val="90000"/>
+                      <a:lumOff val="10000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -1216,7 +1441,10 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="C00000"/>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="90000"/>
+                    <a:lumOff val="10000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1230,7 +1458,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:f>Foglio1!$L$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1253,13 +1481,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1674,6 +1902,24 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$Q$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$B$3:$D$3</c:f>
@@ -1700,11 +1946,11 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$P$3</c:f>
+              <c:f>Foglio1!$P$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1739,7 +1985,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$G$2:$I$2</c:f>
+              <c:f>Foglio1!$Q$2:$S$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1757,7 +2003,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$Q$3:$S$3</c:f>
+              <c:f>Foglio1!$Q$4:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1776,7 +2022,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B098-432C-B0D1-8558A75D0CFB}"/>
+              <c16:uniqueId val="{00000000-C1EC-42DE-A60B-1B63069F71C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1803,7 +2049,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$P$5</c15:sqref>
+                          <c15:sqref>Foglio1!$P$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1844,7 +2090,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$G$2:$I$2</c15:sqref>
+                          <c15:sqref>Foglio1!$Q$2:$S$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1868,7 +2114,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$Q$5:$S$5</c15:sqref>
+                          <c15:sqref>Foglio1!$Q$6:$S$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1904,7 +2150,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$P$4</c15:sqref>
+                          <c15:sqref>Foglio1!$P$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1945,7 +2191,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$G$2:$I$2</c15:sqref>
+                          <c15:sqref>Foglio1!$Q$2:$S$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1969,7 +2215,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Foglio1!$Q$4:$S$4</c15:sqref>
+                          <c15:sqref>Foglio1!$Q$5:$S$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1992,6 +2238,98 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-B098-432C-B0D1-8558A75D0CFB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$P$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>15 thread</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$Q$2:$S$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$Q$3:$S$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-B098-432C-B0D1-8558A75D0CFB}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3915,16 +4253,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>159830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3951,16 +4289,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>547874</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>160499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3990,15 +4328,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>347849</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>160499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4345,15 +4683,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9C14D-E9C5-4D59-B760-E1A9A0956FE3}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -4430,129 +4770,167 @@
         <v>333</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="3">
+        <v>40</v>
+      </c>
+      <c r="I3" s="3">
+        <v>83</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3">
         <v>36</v>
       </c>
-      <c r="I3" s="3">
-        <v>80</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="3">
-        <v>11</v>
-      </c>
-      <c r="M3" s="3">
-        <v>38</v>
-      </c>
       <c r="N3" s="3">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>14</v>
-      </c>
-      <c r="R3" s="3">
-        <v>41</v>
-      </c>
-      <c r="S3" s="3">
-        <v>116</v>
+        <v>9</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="F4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3">
         <v>12</v>
       </c>
       <c r="H4" s="3">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="I4" s="3">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M4" s="3">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N4" s="3">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="3">
         <v>14</v>
       </c>
       <c r="R4" s="3">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="S4" s="3">
-        <v>106</v>
-      </c>
-      <c r="T4" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H5" s="3">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I5" s="3">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M5" s="3">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="N5" s="3">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R5" s="3">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="S5" s="3">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="T5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3">
+        <v>67</v>
+      </c>
+      <c r="I6" s="3">
+        <v>175</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
+        <v>18</v>
+      </c>
+      <c r="M6" s="3">
+        <v>59</v>
+      </c>
+      <c r="N6" s="3">
+        <v>128</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>16</v>
+      </c>
+      <c r="R6" s="3">
+        <v>43</v>
+      </c>
+      <c r="S6" s="3">
+        <v>114</v>
+      </c>
+      <c r="T6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>